<commit_message>
implementation of plot and filesaving
</commit_message>
<xml_diff>
--- a/src/experiment_data.xlsx
+++ b/src/experiment_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezgin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrie\PycharmProjects\OlfactoMeter\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6117B8E-07A4-44D1-BC5F-9E07633A0446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE4326B-93BC-456C-B25D-D04E7D29CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="660" windowWidth="19992" windowHeight="12300" xr2:uid="{28521587-7B25-C546-BEFB-594893D6897F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{28521587-7B25-C546-BEFB-594893D6897F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t>odor1</t>
-  </si>
-  <si>
     <t>purging</t>
-  </si>
-  <si>
-    <t>odor2</t>
   </si>
   <si>
     <t>mode</t>
   </si>
   <si>
     <t>duration</t>
+  </si>
+  <si>
+    <t>odor_2</t>
+  </si>
+  <si>
+    <t>odor_1</t>
   </si>
 </sst>
 </file>
@@ -410,54 +410,54 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2</v>

</xml_diff>